<commit_message>
Updated to have a "document" field
Updated the spreadsheet to explicitly have a field for the specific document to be reviewed (with dropdown list to choose from)
</commit_message>
<xml_diff>
--- a/4_Methodology/CommentsTemplate.xlsx
+++ b/4_Methodology/CommentsTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\be.wood\Documents\cert stuff\Common Criteria\iTCs\Biometric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\be.wood\Documents\GitHub\cPP-biometrics\4_Methodology\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Section</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Proposed Change/Rationale</t>
-  </si>
-  <si>
-    <t>Review Comments Matrix for XYZ</t>
   </si>
   <si>
     <t>#</t>
@@ -167,6 +164,31 @@
   </si>
   <si>
     <t>Email of Reviewer:</t>
+  </si>
+  <si>
+    <t>Review Comments Matrix for:</t>
+  </si>
+  <si>
+    <t>DOCUMENT</t>
+  </si>
+  <si>
+    <t>cPP</t>
+  </si>
+  <si>
+    <t>CFG</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>The specific document the comments are for should be selected in G1. The fields are:
+- cPP - for the PP-Module
+- CFG - for the PP-Configuration
+- SD - for the Supporting Document
+- TB - for the PAD Toolbox overview</t>
   </si>
 </sst>
 </file>
@@ -225,7 +247,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="22"/>
       </patternFill>
     </fill>
@@ -331,11 +353,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,9 +375,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -366,16 +402,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,6 +479,16 @@
     <tableColumn id="8" name="Issue/_x000a_Pull Request" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H7:H11" totalsRowShown="0">
+  <autoFilter ref="H7:H11"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="DOCUMENT"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -756,7 +792,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -770,54 +806,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -825,273 +863,312 @@
         <f>ROW(A1)</f>
         <v>1</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A28" si="0">ROW(A3)</f>
         <v>3</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H28" s="6"/>
+      <c r="H28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Instructions!$H$8:$H$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="96.5" customWidth="1"/>
+    <col min="8" max="8" width="12.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="8" t="s">
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8" t="s">
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
+      <c r="H11" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>